<commit_message>
updated product backlog following sprint 1 demo
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\Dropbox\Work\_teaching\UWG\Capstone\Spring 2022\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lanthorr\git\Capstone\5\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3838CCD7-8993-4A1E-AB80-532D3D0EC31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D053C19-4455-4F52-87F4-719A7F05471B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3630" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C9" sqref="A8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -646,16 +646,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,38 +694,38 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>